<commit_message>
Manejo de errores consulta firestore
</commit_message>
<xml_diff>
--- a/informe-acciones-usd.xlsx
+++ b/informe-acciones-usd.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,29 +512,298 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>AMZN.BA</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1925</v>
+      </c>
+      <c r="D3" t="n">
+        <v>35</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1930</v>
+      </c>
+      <c r="F3" t="n">
+        <v>67550</v>
+      </c>
+      <c r="G3" t="n">
+        <v>175</v>
+      </c>
+      <c r="H3" t="n">
+        <v>45.64</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.1199999999999974</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>COME.BA</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>96.8</v>
+      </c>
+      <c r="D4" t="n">
+        <v>741</v>
+      </c>
+      <c r="E4" t="n">
+        <v>229.25</v>
+      </c>
+      <c r="F4" t="n">
+        <v>169874.25</v>
+      </c>
+      <c r="G4" t="n">
+        <v>98145.45</v>
+      </c>
+      <c r="H4" t="n">
+        <v>114.78</v>
+      </c>
+      <c r="I4" t="n">
+        <v>66.31</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>GGAL.BA</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>3035</v>
+      </c>
+      <c r="D5" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4110</v>
+      </c>
+      <c r="F5" t="n">
+        <v>28770</v>
+      </c>
+      <c r="G5" t="n">
+        <v>7525</v>
+      </c>
+      <c r="H5" t="n">
+        <v>19.44</v>
+      </c>
+      <c r="I5" t="n">
+        <v>5.090000000000002</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>GOOGL.BA</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>3998.94</v>
+      </c>
+      <c r="D6" t="n">
+        <v>17</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4560</v>
+      </c>
+      <c r="F6" t="n">
+        <v>77520</v>
+      </c>
+      <c r="G6" t="n">
+        <v>9538.02</v>
+      </c>
+      <c r="H6" t="n">
+        <v>52.38</v>
+      </c>
+      <c r="I6" t="n">
+        <v>6.450000000000003</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MELI.BA</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>18890.38</v>
+      </c>
+      <c r="D7" t="n">
+        <v>8</v>
+      </c>
+      <c r="E7" t="n">
+        <v>20950</v>
+      </c>
+      <c r="F7" t="n">
+        <v>167600</v>
+      </c>
+      <c r="G7" t="n">
+        <v>16476.96</v>
+      </c>
+      <c r="H7" t="n">
+        <v>113.24</v>
+      </c>
+      <c r="I7" t="n">
+        <v>11.13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>META.BA</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>10900</v>
+      </c>
+      <c r="D8" t="n">
+        <v>9</v>
+      </c>
+      <c r="E8" t="n">
+        <v>29650</v>
+      </c>
+      <c r="F8" t="n">
+        <v>266850</v>
+      </c>
+      <c r="G8" t="n">
+        <v>168750</v>
+      </c>
+      <c r="H8" t="n">
+        <v>180.3</v>
+      </c>
+      <c r="I8" t="n">
+        <v>114.02</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>NVDA.BA</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C9" t="n">
         <v>7163.88</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D9" t="n">
         <v>21</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E9" t="n">
         <v>7690</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F9" t="n">
         <v>161490</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G9" t="n">
         <v>11048.52</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H9" t="n">
         <v>109.11</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I9" t="n">
         <v>7.459999999999994</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>PAMP.BA</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2528</v>
+      </c>
+      <c r="D10" t="n">
+        <v>14</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2690</v>
+      </c>
+      <c r="F10" t="n">
+        <v>37660</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2268</v>
+      </c>
+      <c r="H10" t="n">
+        <v>25.45</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1.539999999999999</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>PFE.BA</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>9267.58</v>
+      </c>
+      <c r="D11" t="n">
+        <v>6</v>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>VIST.BA</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>14377.5</v>
+      </c>
+      <c r="D12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" t="n">
+        <v>22900</v>
+      </c>
+      <c r="F12" t="n">
+        <v>91600</v>
+      </c>
+      <c r="G12" t="n">
+        <v>34090</v>
+      </c>
+      <c r="H12" t="n">
+        <v>61.89</v>
+      </c>
+      <c r="I12" t="n">
+        <v>23.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>